<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2025-10-14.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2025-10-14.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2025-10-14.xlsx
@@ -522,6 +522,9 @@
       <c r="C11" t="str">
         <v>577_腊梅白_wax white_undefined_1bunch</v>
       </c>
+      <c r="F11" t="str">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -583,7 +586,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>058810310202050</v>
+        <v>058810310202055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>